<commit_message>
Outputs mis à jour
</commit_message>
<xml_diff>
--- a/1-Output/Export_Category.xlsx
+++ b/1-Output/Export_Category.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,439 +548,329 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>312</v>
+        <v>1089</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>DAQ-Module</t>
+          <t>Pressure sensor</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>490</v>
+        <v>1130</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>DAQ</t>
+          <t>SHED chamber</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>524</v>
+        <v>1139</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>CAN Interface device</t>
+          <t>FID ppm C3H8</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>548</v>
+        <v>1141</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CAN AD Module</t>
+          <t>Pressure sensor Absolute</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>628</v>
+        <v>1142</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Pressure sensor</t>
+          <t>Pressure sensor relative</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>677</v>
+        <v>1149</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>CAN Module</t>
+          <t xml:space="preserve"> HFID ppmC</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>793</v>
+        <v>1155</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>CAN CNT Module</t>
+          <t>Gas flowmeter C4H10</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>796</v>
+        <v>1156</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>CAN TH Module</t>
+          <t>Gas flowmeter N2</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>827</v>
+        <v>1157</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>CAN TH MiniModule</t>
+          <t>Gas flowmeter Air</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>833</v>
+        <v>1198</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Connector accessory</t>
+          <t>Pressure gauge</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>840</v>
+        <v>1763</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Multifonction test station</t>
+          <t>DAQ-Module</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>859</v>
+        <v>1819</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Terminal Block</t>
+          <t>DAQ</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>877</v>
+        <v>2019</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Shunt</t>
+          <t>DAQ-module</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>1015</v>
+        <v>2268</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>CAN interface device</t>
+          <t>Load sensor - 1 kN</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1130</v>
+        <v>2270</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>SHED chamber</t>
+          <t>Speed sensor</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>1139</v>
+        <v>2273</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>FID ppm C3H8</t>
+          <t>Ball Mass</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>1141</v>
+        <v>2308</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Pressure sensor Absolute</t>
+          <t>Soaking</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>1142</v>
+        <v>2318</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Pressure sensor relative</t>
+          <t>Load sensor - 0,1 kN</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>1149</v>
+        <v>2319</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t xml:space="preserve"> HFID ppmC</t>
+          <t>Calibrated mass</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1155</v>
+        <v>2366</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Gas flowmeter C4H10</t>
+          <t xml:space="preserve">Pressure sensor </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>1156</v>
+        <v>2457</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Gas flowmeter N2</t>
+          <t>Temperature sensor</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>1157</v>
+        <v>2734</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Gas flowmeter Air</t>
+          <t>Volumeter water</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>1198</v>
+        <v>2735</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Pressure gauge</t>
+          <t>Volumeter glycol</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>2019</v>
+        <v>2768</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>DAQ-module</t>
+          <t>Pressure regulator</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>2268</v>
+        <v>2841</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Load sensor - 1 kN</t>
+          <t>Impulse Force Test Hammer</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>2270</v>
+        <v>2842</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Speed sensor</t>
+          <t>Frequency calibrator</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>2273</v>
+        <v>2856</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ball Mass</t>
+          <t>Filter</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>2308</v>
+        <v>2874</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Soaking</t>
+          <t xml:space="preserve">calibration </t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>2318</v>
+        <v>3246</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Load sensor - 0,1 kN</t>
+          <t>Thermometer</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>2319</v>
+        <v>3453</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Calibrated mass</t>
+          <t>Scale</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>2366</v>
+        <v>4092</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t xml:space="preserve">Pressure sensor </t>
+          <t>Flowmeter</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>2457</v>
+        <v>4098</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Temperature sensor</t>
+          <t>Thermocouple</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>2734</v>
+        <v>4169</v>
       </c>
       <c r="B45" t="inlineStr">
-        <is>
-          <t>Volumeter water</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="1" t="n">
-        <v>2735</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>Volumeter glycol</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="1" t="n">
-        <v>2768</v>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>Pressure regulator</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="1" t="n">
-        <v>2841</v>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>Impulse Force Test Hammer</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="1" t="n">
-        <v>2842</v>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>Frequency calibrator</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="1" t="n">
-        <v>2856</v>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>Filter</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="1" t="n">
-        <v>2874</v>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t xml:space="preserve">calibration </t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="1" t="n">
-        <v>3246</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Thermometer</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="1" t="n">
-        <v>3453</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>Scale</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="1" t="n">
-        <v>4092</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Flowmeter</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="1" t="n">
-        <v>4098</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Thermocouple</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="1" t="n">
-        <v>4169</v>
-      </c>
-      <c r="B56" t="inlineStr">
         <is>
           <t>Measuring chain</t>
         </is>

</xml_diff>